<commit_message>
add cors, fix reorder files
</commit_message>
<xml_diff>
--- a/src/tests/eff(1).xlsx
+++ b/src/tests/eff(1).xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Эффективность" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -132,7 +132,7 @@
       <selection pane="topLeft" activeCell="G91" activeCellId="0" sqref="G91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>